<commit_message>
add percent of each SES by street
</commit_message>
<xml_diff>
--- a/analysis/glm_assoc_summary.xlsx
+++ b/analysis/glm_assoc_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalGitHub\BEPIDL\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B522D0-DDB3-4068-A1E9-3083E4E73FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13158CE-4D95-4113-9239-61680FC32283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="0" windowWidth="24015" windowHeight="20880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="720" windowWidth="24015" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="street level" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>term</t>
   </si>
@@ -44,24 +44,6 @@
     <t>(Intercept)</t>
   </si>
   <si>
-    <t>ses_cat_r5</t>
-  </si>
-  <si>
-    <t>ses_cat_r4</t>
-  </si>
-  <si>
-    <t>ses_cat_r3</t>
-  </si>
-  <si>
-    <t>ses_cat_r2</t>
-  </si>
-  <si>
-    <t>ses_cat_r1</t>
-  </si>
-  <si>
-    <t>Street-level Collision ~ SES</t>
-  </si>
-  <si>
     <t>outcome</t>
   </si>
   <si>
@@ -87,6 +69,21 @@
   </si>
   <si>
     <t>outcome: total pedestrian collision count</t>
+  </si>
+  <si>
+    <t>reference level: ses_level = 6</t>
+  </si>
+  <si>
+    <t>ses_level</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>percent_street</t>
+  </si>
+  <si>
+    <t>SES Level by Street, and Association with Pedestrian Collision</t>
   </si>
 </sst>
 </file>
@@ -445,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -699,45 +696,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -778,8 +736,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -791,8 +751,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -804,8 +766,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -817,42 +781,8 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -900,52 +830,61 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="18" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1327,300 +1266,427 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S22" sqref="S22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
-    </row>
-    <row r="2" spans="1:6" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="22" t="s">
+    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="I2" s="21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>6</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="1">
+        <v>100669</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1819</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.8069117603234299</v>
+      </c>
+      <c r="E3" s="1">
         <v>-1.6311114476669899</v>
       </c>
-      <c r="C3" s="18">
+      <c r="F3" s="1">
         <v>9.0995994591152193E-2</v>
       </c>
-      <c r="D3" s="18">
+      <c r="G3" s="1">
         <v>-17.925090604214201</v>
       </c>
-      <c r="E3" s="19">
+      <c r="H3" s="9">
         <v>7.5128050063711197E-72</v>
       </c>
-      <c r="F3" s="20">
+      <c r="I3" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>100669</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2600</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.5827215925458602</v>
+      </c>
+      <c r="E4" s="3">
         <v>6.4954043592788099E-2</v>
       </c>
-      <c r="C4" s="5">
+      <c r="F4" s="3">
         <v>0.11810878420316601</v>
       </c>
-      <c r="D4" s="5">
+      <c r="G4" s="3">
         <v>0.54995099671042602</v>
       </c>
-      <c r="E4" s="5">
+      <c r="H4" s="3">
         <v>0.58235298478368802</v>
       </c>
-      <c r="F4" s="7">
+      <c r="I4" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>100669</v>
+      </c>
+      <c r="C5" s="3">
+        <v>7394</v>
+      </c>
+      <c r="D5" s="3">
+        <v>7.34486286741698</v>
+      </c>
+      <c r="E5" s="3">
         <v>0.21265820700702301</v>
       </c>
-      <c r="C5" s="5">
+      <c r="F5" s="3">
         <v>0.100920374177907</v>
       </c>
-      <c r="D5" s="5">
+      <c r="G5" s="3">
         <v>2.1071880553290199</v>
       </c>
-      <c r="E5" s="5">
+      <c r="H5" s="3">
         <v>3.5101281900204201E-2</v>
       </c>
-      <c r="F5" s="7">
+      <c r="I5" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="5">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>100669</v>
+      </c>
+      <c r="C6" s="3">
+        <v>34547</v>
+      </c>
+      <c r="D6" s="3">
+        <v>34.317416483723797</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.34846832388807603</v>
       </c>
-      <c r="C6" s="5">
+      <c r="F6" s="3">
         <v>9.31275151855291E-2</v>
       </c>
-      <c r="D6" s="5">
+      <c r="G6" s="3">
         <v>3.7418406707604599</v>
       </c>
-      <c r="E6" s="6">
+      <c r="H6" s="4">
         <v>1.8267732556893101E-4</v>
       </c>
-      <c r="F6" s="7">
+      <c r="I6" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="5">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="23">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100669</v>
+      </c>
+      <c r="C7" s="3">
+        <v>40763</v>
+      </c>
+      <c r="D7" s="3">
+        <v>40.492107798825799</v>
+      </c>
+      <c r="E7" s="3">
         <v>-6.9658111132699402E-2</v>
       </c>
-      <c r="C7" s="5">
+      <c r="F7" s="3">
         <v>9.3052732262962706E-2</v>
       </c>
-      <c r="D7" s="5">
+      <c r="G7" s="3">
         <v>-0.74858748839151501</v>
       </c>
-      <c r="E7" s="5">
+      <c r="H7" s="3">
         <v>0.454105875486703</v>
       </c>
-      <c r="F7" s="7">
+      <c r="I7" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="13">
+    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>100669</v>
+      </c>
+      <c r="C8" s="6">
+        <v>13546</v>
+      </c>
+      <c r="D8" s="6">
+        <v>13.4559794971639</v>
+      </c>
+      <c r="E8" s="6">
         <v>-1.1269662101222699</v>
       </c>
-      <c r="C8" s="13">
+      <c r="F8" s="6">
         <v>0.10089160809909101</v>
       </c>
-      <c r="D8" s="13">
+      <c r="G8" s="6">
         <v>-11.170068862569901</v>
       </c>
-      <c r="E8" s="14">
+      <c r="H8" s="7">
         <v>5.7136567427544401E-29</v>
       </c>
-      <c r="F8" s="15">
+      <c r="I8" s="8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="22">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
+        <v>100818</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1646</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.6326449641929</v>
+      </c>
+      <c r="E9" s="1">
         <v>-1.60398500586115</v>
       </c>
-      <c r="C9" s="2">
+      <c r="F9" s="1">
         <v>9.5550422599697996E-2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="G9" s="1">
         <v>-16.786791331953999</v>
       </c>
-      <c r="E9" s="16">
+      <c r="H9" s="9">
         <v>3.04889073441289E-63</v>
       </c>
-      <c r="F9" s="3">
+      <c r="I9" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>100818</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2466</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.4459917871808599</v>
+      </c>
+      <c r="E10" s="3">
         <v>0.16865714196621501</v>
       </c>
-      <c r="C10" s="5">
+      <c r="F10" s="3">
         <v>0.122110217784798</v>
       </c>
-      <c r="D10" s="5">
+      <c r="G10" s="3">
         <v>1.3811877910450401</v>
       </c>
-      <c r="E10" s="5">
+      <c r="H10" s="3">
         <v>0.16722122769202399</v>
       </c>
-      <c r="F10" s="7">
+      <c r="I10" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>100818</v>
+      </c>
+      <c r="C11" s="3">
+        <v>7901</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7.8368942053998198</v>
+      </c>
+      <c r="E11" s="3">
         <v>0.17779637231001499</v>
       </c>
-      <c r="C11" s="5">
+      <c r="F11" s="3">
         <v>0.104543649281439</v>
       </c>
-      <c r="D11" s="5">
+      <c r="G11" s="3">
         <v>1.7006903196135199</v>
       </c>
-      <c r="E11" s="5">
+      <c r="H11" s="3">
         <v>8.9001153843136796E-2</v>
       </c>
-      <c r="F11" s="7">
+      <c r="I11" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>100818</v>
+      </c>
+      <c r="C12" s="3">
+        <v>35699</v>
+      </c>
+      <c r="D12" s="3">
+        <v>35.4093515046916</v>
+      </c>
+      <c r="E12" s="3">
         <v>0.30530876405864998</v>
       </c>
-      <c r="C12" s="5">
+      <c r="F12" s="3">
         <v>9.7540717265142796E-2</v>
       </c>
-      <c r="D12" s="5">
+      <c r="G12" s="3">
         <v>3.13006478339436</v>
       </c>
-      <c r="E12" s="5">
+      <c r="H12" s="3">
         <v>1.74767756184783E-3</v>
       </c>
-      <c r="F12" s="7">
+      <c r="I12" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="5">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>100818</v>
+      </c>
+      <c r="C13" s="3">
+        <v>41189</v>
+      </c>
+      <c r="D13" s="3">
+        <v>40.854807673232898</v>
+      </c>
+      <c r="E13" s="3">
         <v>-0.134703149242036</v>
       </c>
-      <c r="C13" s="5">
+      <c r="F13" s="3">
         <v>9.7530210353534194E-2</v>
       </c>
-      <c r="D13" s="5">
+      <c r="G13" s="3">
         <v>-1.38114281465973</v>
       </c>
-      <c r="E13" s="5">
+      <c r="H13" s="3">
         <v>0.167235053506122</v>
       </c>
-      <c r="F13" s="7">
+      <c r="I13" s="5">
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="9">
+    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6">
+        <v>100818</v>
+      </c>
+      <c r="C14" s="6">
+        <v>11917</v>
+      </c>
+      <c r="D14" s="6">
+        <v>11.8203098653018</v>
+      </c>
+      <c r="E14" s="6">
         <v>-1.08346817111286</v>
       </c>
-      <c r="C14" s="9">
+      <c r="F14" s="6">
         <v>0.105861606225806</v>
       </c>
-      <c r="D14" s="9">
+      <c r="G14" s="6">
         <v>-10.234760360633301</v>
       </c>
-      <c r="E14" s="10">
+      <c r="H14" s="7">
         <v>1.3853773089643E-24</v>
       </c>
-      <c r="F14" s="11">
+      <c r="I14" s="8">
         <v>500</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>21</v>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1630,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0898E-2C65-458B-81DF-E90E3BAB7A2D}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,273 +1710,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="F2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.8254432971942798</v>
+      </c>
+      <c r="C3" s="3">
+        <v>7.2478990622841702E-2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>38.982928334322601</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.26898258062763403</v>
+      </c>
+      <c r="C4" s="3">
+        <v>9.3241720225644503E-2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.8847878393566502</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3.9167752116095501E-3</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.28537087203689199</v>
+      </c>
+      <c r="C5" s="3">
+        <v>9.8912398115114403E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.88508698075217</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3.9130553253180099E-3</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.19921032240477701</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.1075918731405595E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.1872996196972099</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.8720658486024401E-2</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.7564225670620801</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.2580678057454398E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>37.977360377924803</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.271674990993927</v>
+      </c>
+      <c r="C8" s="3">
+        <v>9.3346926056885507E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.91037961794658</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3.6099000085916201E-3</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.27479959147384497</v>
+      </c>
+      <c r="C9" s="3">
+        <v>9.9036495514810696E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.7747305682151202</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5.5247456843345501E-3</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.18149243381701199</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9.1207830618599203E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1.98987776143863</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.6604402669875498E-2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.4113291570482496E-2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.108298445652822</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.86901793468195798</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.384837321216353</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2.8254432971942798</v>
-      </c>
-      <c r="C3" s="5">
-        <v>7.2478990622841702E-2</v>
-      </c>
-      <c r="D3" s="5">
-        <v>38.982928334322601</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.26898258062763403</v>
-      </c>
-      <c r="C4" s="5">
-        <v>9.3241720225644503E-2</v>
-      </c>
-      <c r="D4" s="5">
-        <v>2.8847878393566502</v>
-      </c>
-      <c r="E4" s="5">
-        <v>3.9167752116095501E-3</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0.28537087203689199</v>
-      </c>
-      <c r="C5" s="5">
-        <v>9.8912398115114403E-2</v>
-      </c>
-      <c r="D5" s="5">
-        <v>2.88508698075217</v>
-      </c>
-      <c r="E5" s="5">
-        <v>3.9130553253180099E-3</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.19921032240477701</v>
-      </c>
-      <c r="C6" s="5">
-        <v>9.1075918731405595E-2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2.1872996196972099</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2.8720658486024401E-2</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2.7564225670620801</v>
-      </c>
-      <c r="C7" s="5">
-        <v>7.2580678057454398E-2</v>
-      </c>
-      <c r="D7" s="5">
-        <v>37.977360377924803</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0.271674990993927</v>
-      </c>
-      <c r="C8" s="5">
-        <v>9.3346926056885507E-2</v>
-      </c>
-      <c r="D8" s="5">
-        <v>2.91037961794658</v>
-      </c>
-      <c r="E8" s="5">
-        <v>3.6099000085916201E-3</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="5">
-        <v>0.27479959147384497</v>
-      </c>
-      <c r="C9" s="5">
-        <v>9.9036495514810696E-2</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2.7747305682151202</v>
-      </c>
-      <c r="E9" s="5">
-        <v>5.5247456843345501E-3</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="5">
-        <v>0.18149243381701199</v>
-      </c>
-      <c r="C10" s="5">
-        <v>9.1207830618599203E-2</v>
-      </c>
-      <c r="D10" s="5">
-        <v>1.98987776143863</v>
-      </c>
-      <c r="E10" s="5">
-        <v>4.6604402669875498E-2</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="5">
-        <v>9.4113291570482496E-2</v>
-      </c>
-      <c r="C11" s="5">
-        <v>0.108298445652822</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.86901793468195798</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.384837321216353</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="5">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3">
         <v>0.22911371830070801</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>0.13685823367849601</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>1.67409524544161</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>9.4111882055298399E-2</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>19</v>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3">
         <v>0.43957047027155999</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>0.14199326042328</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <v>3.09571362021833</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>1.96339888745584E-3</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>19</v>
+      <c r="F13" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="5">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3">
         <v>0.42899184182556799</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>0.13185538370328001</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <v>3.25350266160497</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>1.13991657440964E-3</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>19</v>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update nb profile distribution in zat profile-collision assoc
</commit_message>
<xml_diff>
--- a/analysis/glm_assoc_summary.xlsx
+++ b/analysis/glm_assoc_summary.xlsx
@@ -8,23 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalGitHub\BEPIDL\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13158CE-4D95-4113-9239-61680FC32283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFA4773-DC3B-4CBE-8475-017D81B262A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="720" windowWidth="24015" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24345" yWindow="0" windowWidth="24015" windowHeight="20880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="street level" sheetId="1" r:id="rId1"/>
-    <sheet name="ZAT level" sheetId="2" r:id="rId2"/>
+    <sheet name="street SES-collision" sheetId="1" r:id="rId1"/>
+    <sheet name="ZAT profile-collision" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
-  <si>
-    <t>term</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>estimate</t>
   </si>
@@ -41,31 +38,16 @@
     <t>buffer_m</t>
   </si>
   <si>
-    <t>(Intercept)</t>
-  </si>
-  <si>
     <t>outcome</t>
   </si>
   <si>
     <t>total</t>
   </si>
   <si>
-    <t>clus2</t>
-  </si>
-  <si>
-    <t>clus3</t>
-  </si>
-  <si>
-    <t>clus4</t>
-  </si>
-  <si>
     <t>injury</t>
   </si>
   <si>
     <t>death</t>
-  </si>
-  <si>
-    <t>ZAT-level Collision ~ Profile (Cluster)</t>
   </si>
   <si>
     <t>outcome: total pedestrian collision count</t>
@@ -84,6 +66,18 @@
   </si>
   <si>
     <t>SES Level by Street, and Association with Pedestrian Collision</t>
+  </si>
+  <si>
+    <t>nb_profile</t>
+  </si>
+  <si>
+    <t>percent_zat</t>
+  </si>
+  <si>
+    <t>Neighborhood (ZAT) Profile Distribution, and Association with Pedestrian Collision</t>
+  </si>
+  <si>
+    <t>reference level: nb_profile = 1</t>
   </si>
 </sst>
 </file>
@@ -442,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -782,6 +776,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -830,7 +837,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -841,28 +848,13 @@
     <xf numFmtId="11" fontId="18" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -886,6 +878,25 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1268,13 +1279,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" customWidth="1"/>
@@ -1285,49 +1296,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
-    </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="A1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="H2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="I2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="17">
         <v>6</v>
       </c>
       <c r="B3" s="1">
@@ -1356,7 +1367,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="23">
+      <c r="A4" s="18">
         <v>5</v>
       </c>
       <c r="B4" s="3">
@@ -1385,7 +1396,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="3">
@@ -1414,7 +1425,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
+      <c r="A6" s="18">
         <v>3</v>
       </c>
       <c r="B6" s="3">
@@ -1443,7 +1454,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="18">
         <v>2</v>
       </c>
       <c r="B7" s="3">
@@ -1472,7 +1483,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="24">
+      <c r="A8" s="19">
         <v>1</v>
       </c>
       <c r="B8" s="6">
@@ -1501,7 +1512,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="17">
         <v>6</v>
       </c>
       <c r="B9" s="1">
@@ -1530,7 +1541,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="23">
+      <c r="A10" s="18">
         <v>5</v>
       </c>
       <c r="B10" s="3">
@@ -1559,7 +1570,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="23">
+      <c r="A11" s="18">
         <v>4</v>
       </c>
       <c r="B11" s="3">
@@ -1588,7 +1599,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="18">
         <v>3</v>
       </c>
       <c r="B12" s="3">
@@ -1617,7 +1628,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="23">
+      <c r="A13" s="18">
         <v>2</v>
       </c>
       <c r="B13" s="3">
@@ -1646,7 +1657,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24">
+      <c r="A14" s="19">
         <v>1</v>
       </c>
       <c r="B14" s="6">
@@ -1675,13 +1686,13 @@
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>16</v>
+      <c r="A17" s="12" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>15</v>
+      <c r="A18" s="13" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1694,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0898E-2C65-458B-81DF-E90E3BAB7A2D}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1705,283 +1716,431 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-    </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:9" s="24" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="H2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="I2" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>172</v>
+      </c>
+      <c r="C3" s="1">
+        <v>863</v>
+      </c>
+      <c r="D3" s="1">
+        <v>19.9304750869061</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.8254432971942798</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.2478990622841702E-2</v>
+      </c>
+      <c r="G3" s="1">
+        <v>38.982928334322601</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>238</v>
+      </c>
+      <c r="C4" s="3">
+        <v>863</v>
+      </c>
+      <c r="D4" s="3">
+        <v>27.578215527230501</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.26898258062763403</v>
+      </c>
+      <c r="F4" s="3">
+        <v>9.3241720225644503E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.8847878393566502</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3.9167752116095501E-3</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>181</v>
+      </c>
+      <c r="C5" s="3">
+        <v>863</v>
+      </c>
+      <c r="D5" s="3">
+        <v>20.973348783314002</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.28537087203689199</v>
+      </c>
+      <c r="F5" s="3">
+        <v>9.8912398115114403E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.88508698075217</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3.9130553253180099E-3</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="B6" s="6">
+        <v>272</v>
+      </c>
+      <c r="C6" s="6">
+        <v>863</v>
+      </c>
+      <c r="D6" s="6">
+        <v>31.517960602549199</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.19921032240477701</v>
+      </c>
+      <c r="F6" s="6">
+        <v>9.1075918731405595E-2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2.1872996196972099</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.8720658486024401E-2</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>172</v>
+      </c>
+      <c r="C7" s="1">
+        <v>863</v>
+      </c>
+      <c r="D7" s="1">
+        <v>19.9304750869061</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.7564225670620801</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7.2580678057454398E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>37.977360377924803</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
-        <v>2.8254432971942798</v>
-      </c>
-      <c r="C3" s="3">
-        <v>7.2478990622841702E-2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>38.982928334322601</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3" t="s">
+    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <v>238</v>
+      </c>
+      <c r="C8" s="3">
+        <v>863</v>
+      </c>
+      <c r="D8" s="3">
+        <v>27.578215527230501</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.271674990993927</v>
+      </c>
+      <c r="F8" s="3">
+        <v>9.3346926056885507E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.91037961794658</v>
+      </c>
+      <c r="H8" s="3">
+        <v>3.6099000085916201E-3</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>181</v>
+      </c>
+      <c r="C9" s="3">
+        <v>863</v>
+      </c>
+      <c r="D9" s="3">
+        <v>20.973348783314002</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.27479959147384497</v>
+      </c>
+      <c r="F9" s="3">
+        <v>9.9036495514810696E-2</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.7747305682151202</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5.5247456843345501E-3</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28">
+        <v>4</v>
+      </c>
+      <c r="B10" s="6">
+        <v>272</v>
+      </c>
+      <c r="C10" s="6">
+        <v>863</v>
+      </c>
+      <c r="D10" s="6">
+        <v>31.517960602549199</v>
+      </c>
+      <c r="E10" s="6">
+        <v>0.18149243381701199</v>
+      </c>
+      <c r="F10" s="6">
+        <v>9.1207830618599203E-2</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1.98987776143863</v>
+      </c>
+      <c r="H10" s="6">
+        <v>4.6604402669875498E-2</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1">
+        <v>172</v>
+      </c>
+      <c r="C11" s="1">
+        <v>863</v>
+      </c>
+      <c r="D11" s="1">
+        <v>19.9304750869061</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9.4113291570482496E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.108298445652822</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.86901793468195798</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.384837321216353</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3">
-        <v>0.26898258062763403</v>
-      </c>
-      <c r="C4" s="3">
-        <v>9.3241720225644503E-2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.8847878393566502</v>
-      </c>
-      <c r="E4" s="3">
-        <v>3.9167752116095501E-3</v>
-      </c>
-      <c r="F4" s="3" t="s">
+    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <v>2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>238</v>
+      </c>
+      <c r="C12" s="3">
+        <v>863</v>
+      </c>
+      <c r="D12" s="3">
+        <v>27.578215527230501</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.22911371830070801</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.13685823367849601</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1.67409524544161</v>
+      </c>
+      <c r="H12" s="3">
+        <v>9.4111882055298399E-2</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="3">
-        <v>0.28537087203689199</v>
-      </c>
-      <c r="C5" s="3">
-        <v>9.8912398115114403E-2</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2.88508698075217</v>
-      </c>
-      <c r="E5" s="3">
-        <v>3.9130553253180099E-3</v>
-      </c>
-      <c r="F5" s="3" t="s">
+    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3">
+        <v>181</v>
+      </c>
+      <c r="C13" s="3">
+        <v>863</v>
+      </c>
+      <c r="D13" s="3">
+        <v>20.973348783314002</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.43957047027155999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.14199326042328</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3.09571362021833</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.96339888745584E-3</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3">
-        <v>0.19921032240477701</v>
-      </c>
-      <c r="C6" s="3">
-        <v>9.1075918731405595E-2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2.1872996196972099</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.8720658486024401E-2</v>
-      </c>
-      <c r="F6" s="3" t="s">
+    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="28">
+        <v>4</v>
+      </c>
+      <c r="B14" s="6">
+        <v>272</v>
+      </c>
+      <c r="C14" s="6">
+        <v>863</v>
+      </c>
+      <c r="D14" s="6">
+        <v>31.517960602549199</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.42899184182556799</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.13185538370328001</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3.25350266160497</v>
+      </c>
+      <c r="H14" s="6">
+        <v>1.13991657440964E-3</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2.7564225670620801</v>
-      </c>
-      <c r="C7" s="3">
-        <v>7.2580678057454398E-2</v>
-      </c>
-      <c r="D7" s="3">
-        <v>37.977360377924803</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.271674990993927</v>
-      </c>
-      <c r="C8" s="3">
-        <v>9.3346926056885507E-2</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.91037961794658</v>
-      </c>
-      <c r="E8" s="3">
-        <v>3.6099000085916201E-3</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.27479959147384497</v>
-      </c>
-      <c r="C9" s="3">
-        <v>9.9036495514810696E-2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2.7747305682151202</v>
-      </c>
-      <c r="E9" s="3">
-        <v>5.5247456843345501E-3</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.18149243381701199</v>
-      </c>
-      <c r="C10" s="3">
-        <v>9.1207830618599203E-2</v>
-      </c>
-      <c r="D10" s="3">
-        <v>1.98987776143863</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4.6604402669875498E-2</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3">
-        <v>9.4113291570482496E-2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.108298445652822</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.86901793468195798</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.384837321216353</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3">
-        <v>0.22911371830070801</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.13685823367849601</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1.67409524544161</v>
-      </c>
-      <c r="E12" s="3">
-        <v>9.4111882055298399E-2</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="3">
-        <v>0.43957047027155999</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.14199326042328</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3.09571362021833</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1.96339888745584E-3</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3">
-        <v>0.42899184182556799</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.13185538370328001</v>
-      </c>
-      <c r="D14" s="3">
-        <v>3.25350266160497</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.13991657440964E-3</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
+    <row r="15" spans="1:9" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
assoc. collision-ses at ZAT level
</commit_message>
<xml_diff>
--- a/analysis/glm_assoc_summary.xlsx
+++ b/analysis/glm_assoc_summary.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LocalGitHub\BEPIDL\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hx83/Documents/GitHub/BEPIDL/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFA4773-DC3B-4CBE-8475-017D81B262A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974F04CE-1A78-A54B-9EE0-ADBF11A994EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24345" yWindow="0" windowWidth="24015" windowHeight="20880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34240" yWindow="780" windowWidth="34560" windowHeight="20020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="street SES-collision" sheetId="1" r:id="rId1"/>
     <sheet name="ZAT profile-collision" sheetId="2" r:id="rId2"/>
+    <sheet name="ZAT SES-collision" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="20">
   <si>
     <t>estimate</t>
   </si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>reference level: nb_profile = 1</t>
+  </si>
+  <si>
+    <t>SES level by ZAT, and Association with Pedestrian Collision</t>
   </si>
 </sst>
 </file>
@@ -837,7 +841,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
@@ -878,6 +882,13 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -887,16 +898,27 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1283,32 +1305,32 @@
       <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="11" customWidth="1"/>
+    <col min="2" max="2" width="7.5" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="22"/>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -1337,7 +1359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="17">
         <v>6</v>
       </c>
@@ -1366,7 +1388,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>5</v>
       </c>
@@ -1395,7 +1417,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>4</v>
       </c>
@@ -1424,7 +1446,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -1453,7 +1475,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>2</v>
       </c>
@@ -1482,7 +1504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19">
         <v>1</v>
       </c>
@@ -1511,7 +1533,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="17">
         <v>6</v>
       </c>
@@ -1540,7 +1562,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>5</v>
       </c>
@@ -1569,7 +1591,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>4</v>
       </c>
@@ -1598,7 +1620,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>3</v>
       </c>
@@ -1627,7 +1649,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>2</v>
       </c>
@@ -1656,7 +1678,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19">
         <v>1</v>
       </c>
@@ -1685,12 +1707,12 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
         <v>9</v>
       </c>
@@ -1707,35 +1729,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0898E-2C65-458B-81DF-E90E3BAB7A2D}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="1:9" s="24" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" s="21" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
@@ -1764,8 +1786,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+    <row r="3" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -1789,12 +1811,12 @@
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27">
+    <row r="4" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
         <v>2</v>
       </c>
       <c r="B4" s="3">
@@ -1818,12 +1840,12 @@
       <c r="H4" s="3">
         <v>3.9167752116095501E-3</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27">
+    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
         <v>3</v>
       </c>
       <c r="B5" s="3">
@@ -1847,12 +1869,12 @@
       <c r="H5" s="3">
         <v>3.9130553253180099E-3</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="30" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="28">
+    <row r="6" spans="1:9" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
       <c r="B6" s="6">
@@ -1876,12 +1898,12 @@
       <c r="H6" s="6">
         <v>2.8720658486024401E-2</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+    <row r="7" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22">
         <v>1</v>
       </c>
       <c r="B7" s="1">
@@ -1905,12 +1927,12 @@
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27">
+    <row r="8" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
         <v>2</v>
       </c>
       <c r="B8" s="3">
@@ -1934,12 +1956,12 @@
       <c r="H8" s="3">
         <v>3.6099000085916201E-3</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27">
+    <row r="9" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
         <v>3</v>
       </c>
       <c r="B9" s="3">
@@ -1963,12 +1985,12 @@
       <c r="H9" s="3">
         <v>5.5247456843345501E-3</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="28">
+    <row r="10" spans="1:9" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24">
         <v>4</v>
       </c>
       <c r="B10" s="6">
@@ -1992,12 +2014,12 @@
       <c r="H10" s="6">
         <v>4.6604402669875498E-2</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+    <row r="11" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22">
         <v>1</v>
       </c>
       <c r="B11" s="1">
@@ -2021,12 +2043,12 @@
       <c r="H11" s="1">
         <v>0.384837321216353</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="29" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27">
+    <row r="12" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
         <v>2</v>
       </c>
       <c r="B12" s="3">
@@ -2050,12 +2072,12 @@
       <c r="H12" s="3">
         <v>9.4111882055298399E-2</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="27">
+    <row r="13" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
         <v>3</v>
       </c>
       <c r="B13" s="3">
@@ -2079,12 +2101,12 @@
       <c r="H13" s="3">
         <v>1.96339888745584E-3</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="30" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="28">
+    <row r="14" spans="1:9" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
         <v>4</v>
       </c>
       <c r="B14" s="6">
@@ -2108,36 +2130,626 @@
       <c r="H14" s="6">
         <v>1.13991657440964E-3</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+    <row r="15" spans="1:9" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="23" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" s="20" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0EAC540-0DA2-5A4F-A076-2AD68FD78D2E}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="34"/>
+    </row>
+    <row r="2" spans="1:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="22">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1">
+        <v>877</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3.8768529076396798</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.2639159518349001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.164765244795645</v>
+      </c>
+      <c r="G3" s="1">
+        <v>13.7402518027559</v>
+      </c>
+      <c r="H3" s="1">
+        <v>5.8272770938250699E-43</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>48</v>
+      </c>
+      <c r="C4" s="3">
+        <v>877</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.4732041049030702</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.112096609713962</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.21361159122426901</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.52476838485919497</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.59974421181905901</v>
+      </c>
+      <c r="I4" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>118</v>
+      </c>
+      <c r="C5" s="3">
+        <v>877</v>
+      </c>
+      <c r="D5" s="3">
+        <v>13.45496009122</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.46690335752859502</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.184261120634301</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.5339222724865902</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.12793747922765E-2</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>335</v>
+      </c>
+      <c r="C6" s="3">
+        <v>877</v>
+      </c>
+      <c r="D6" s="3">
+        <v>38.198403648802703</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.88285084549934101</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.17139307636680501</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5.1510298094534201</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2.5906000423122798E-7</v>
+      </c>
+      <c r="I6" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3">
+        <v>261</v>
+      </c>
+      <c r="C7" s="3">
+        <v>877</v>
+      </c>
+      <c r="D7" s="3">
+        <v>29.760547320410399</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.95546183907746995</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.17370670097465099</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5.5004316685335901</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3.7886255891555597E-8</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24">
+        <v>1</v>
+      </c>
+      <c r="B8" s="6">
+        <v>81</v>
+      </c>
+      <c r="C8" s="6">
+        <v>877</v>
+      </c>
+      <c r="D8" s="6">
+        <v>9.2360319270239408</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0.23602857531763899</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0.196837402507273</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.19910429781716</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0.230487393160976</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="22">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>34</v>
+      </c>
+      <c r="C9" s="1">
+        <v>877</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3.8768529076396798</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2.1700384370320598</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.165502931836496</v>
+      </c>
+      <c r="G9" s="1">
+        <v>13.111782449726499</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2.8189432353502001E-39</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3">
+        <v>877</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5.4732041049030702</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.151415140266355</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.21429476053386201</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.70657415929881995</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.47983115208071597</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>118</v>
+      </c>
+      <c r="C11" s="3">
+        <v>877</v>
+      </c>
+      <c r="D11" s="3">
+        <v>13.45496009122</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.48512230014976498</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.18496913633581599</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2.6227202535509</v>
+      </c>
+      <c r="H11" s="3">
+        <v>8.7230864309910793E-3</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3">
+        <v>335</v>
+      </c>
+      <c r="C12" s="3">
+        <v>877</v>
+      </c>
+      <c r="D12" s="3">
+        <v>38.198403648802703</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.89200417663134401</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.17210802401838601</v>
+      </c>
+      <c r="G12" s="3">
+        <v>5.1828157444655103</v>
+      </c>
+      <c r="H12" s="3">
+        <v>2.1856093020766501E-7</v>
+      </c>
+      <c r="I12" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>261</v>
+      </c>
+      <c r="C13" s="3">
+        <v>877</v>
+      </c>
+      <c r="D13" s="3">
+        <v>29.760547320410399</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.98276910585801103</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.17440161698562501</v>
+      </c>
+      <c r="G13" s="3">
+        <v>5.6350917086910499</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.7496520211878599E-8</v>
+      </c>
+      <c r="I13" s="30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6">
+        <v>81</v>
+      </c>
+      <c r="C14" s="6">
+        <v>877</v>
+      </c>
+      <c r="D14" s="6">
+        <v>9.2360319270239408</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.26038002747186501</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.19756060497328401</v>
+      </c>
+      <c r="G14" s="6">
+        <v>1.31797545116384</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.18751186591490401</v>
+      </c>
+      <c r="I14" s="31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="22">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>34</v>
+      </c>
+      <c r="C15" s="1">
+        <v>877</v>
+      </c>
+      <c r="D15" s="1">
+        <v>3.8768529076396798</v>
+      </c>
+      <c r="E15" s="1">
+        <v>-0.23180161405729599</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.26714414520067298</v>
+      </c>
+      <c r="G15" s="1">
+        <v>-0.86770239296530705</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.38555727552815799</v>
+      </c>
+      <c r="I15" s="29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>48</v>
+      </c>
+      <c r="C16" s="3">
+        <v>877</v>
+      </c>
+      <c r="D16" s="3">
+        <v>5.4732041049030702</v>
+      </c>
+      <c r="E16" s="3">
+        <v>-0.32781417387811301</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.36371483919255798</v>
+      </c>
+      <c r="G16" s="3">
+        <v>-0.90129447180614197</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.36743177230281299</v>
+      </c>
+      <c r="I16" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="23">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <v>118</v>
+      </c>
+      <c r="C17" s="3">
+        <v>877</v>
+      </c>
+      <c r="D17" s="3">
+        <v>13.45496009122</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.31881299104691802</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.295044998571934</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1.0805571780237699</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.27989413955451897</v>
+      </c>
+      <c r="I17" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="23">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3">
+        <v>335</v>
+      </c>
+      <c r="C18" s="3">
+        <v>877</v>
+      </c>
+      <c r="D18" s="3">
+        <v>38.198403648802703</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.85178421875989996</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.27476712131528502</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3.1000223559590601</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1.93506036575186E-3</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="23">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3">
+        <v>261</v>
+      </c>
+      <c r="C19" s="3">
+        <v>877</v>
+      </c>
+      <c r="D19" s="3">
+        <v>29.760547320410399</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.69813743725248401</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.278162784726734</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2.5098161061995699</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1.2079404819852001E-2</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="24">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
+        <v>81</v>
+      </c>
+      <c r="C20" s="6">
+        <v>877</v>
+      </c>
+      <c r="D20" s="6">
+        <v>9.2360319270239408</v>
+      </c>
+      <c r="E20" s="6">
+        <v>1.2438785582990899E-2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.32013688438177101</v>
+      </c>
+      <c r="G20" s="6">
+        <v>3.8854584366346603E-2</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0.96900632562896105</v>
+      </c>
+      <c r="I20" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>

</xml_diff>